<commit_message>
added screenshots of Git
</commit_message>
<xml_diff>
--- a/images/hometask.xlsx
+++ b/images/hometask.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="16275" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="16275" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="git" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>mvn compile</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>test results (one test is expected to fail)</t>
+  </si>
+  <si>
+    <t>older screnshot (when working on different machine)</t>
   </si>
 </sst>
 </file>
@@ -91,14 +94,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>132531</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85329</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9129</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -115,8 +118,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="285750" y="152400"/>
+          <a:off x="285750" y="266700"/>
           <a:ext cx="6552381" cy="3171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="3542" r="44680" b="3970"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485775" y="3952875"/>
+          <a:ext cx="9467850" cy="9877425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -835,14 +875,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -881,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>